<commit_message>
Added EEPROM but auto mode messed up rip
</commit_message>
<xml_diff>
--- a/drivers/eeprom/EEPROM format.xlsx
+++ b/drivers/eeprom/EEPROM format.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="5805"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="18">
   <si>
     <t>Address</t>
   </si>
@@ -42,13 +42,37 @@
     <t>_PROM_LCD_BRIGHTNESS</t>
   </si>
   <si>
-    <t>24LC02</t>
+    <t>Size(byte)</t>
   </si>
   <si>
-    <t>Page_Size (bit)</t>
+    <t>Page_Size (bytes)</t>
   </si>
   <si>
-    <t>Size(byte)</t>
+    <t>24LC02H/B</t>
+  </si>
+  <si>
+    <t>16 for H, 8 for B</t>
+  </si>
+  <si>
+    <t>pitch</t>
+  </si>
+  <si>
+    <t>roll</t>
+  </si>
+  <si>
+    <t>shootspeed</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>_PROM_RED_POSSTATE_BASE</t>
+  </si>
+  <si>
+    <t>_PROM_BLUE_POSSTATE_BASE</t>
   </si>
 </sst>
 </file>
@@ -64,12 +88,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0066"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -84,10 +120,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -95,6 +137,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0066"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -406,23 +453,24 @@
   <dimension ref="A1:E258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G143" sqref="G143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -441,8 +489,8 @@
       <c r="A3">
         <v>256</v>
       </c>
-      <c r="B3">
-        <v>16</v>
+      <c r="B3" t="s">
+        <v>10</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -685,1042 +733,1448 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C49">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C50">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C51">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C52">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C53">
         <v>50</v>
       </c>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C54">
         <v>51</v>
       </c>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C55">
         <v>52</v>
       </c>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D55" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C56">
         <v>53</v>
       </c>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C57">
         <v>54</v>
       </c>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C58">
         <v>55</v>
       </c>
-    </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C59">
         <v>56</v>
       </c>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D59" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C60">
         <v>57</v>
       </c>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C61">
         <v>58</v>
       </c>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D61" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C62">
         <v>59</v>
       </c>
-    </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C63">
         <v>60</v>
       </c>
-    </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D63" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C64">
         <v>61</v>
       </c>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C65">
         <v>62</v>
       </c>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D65" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C66">
         <v>63</v>
       </c>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C67">
         <v>64</v>
       </c>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D67" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C68">
         <v>65</v>
       </c>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C69">
         <v>66</v>
       </c>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C70">
         <v>67</v>
       </c>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C71">
         <v>68</v>
       </c>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D71" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C72">
         <v>69</v>
       </c>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C73">
         <v>70</v>
       </c>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D73" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C74">
         <v>71</v>
       </c>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C75">
         <v>72</v>
       </c>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D75" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C76">
         <v>73</v>
       </c>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C77">
         <v>74</v>
       </c>
-    </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D77" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C78">
         <v>75</v>
       </c>
-    </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C79">
         <v>76</v>
       </c>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D79" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C80">
         <v>77</v>
       </c>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C81">
         <v>78</v>
       </c>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D81" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C82">
         <v>79</v>
       </c>
-    </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C83">
         <v>80</v>
       </c>
-    </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D83" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C84">
         <v>81</v>
       </c>
-    </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C85">
         <v>82</v>
       </c>
-    </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D85" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C86">
         <v>83</v>
       </c>
-    </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C87">
         <v>84</v>
       </c>
-    </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D87" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C88">
         <v>85</v>
       </c>
-    </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C89">
         <v>86</v>
       </c>
-    </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D89" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C90">
         <v>87</v>
       </c>
-    </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D90" s="2"/>
+    </row>
+    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C91">
         <v>88</v>
       </c>
-    </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D91" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C92">
         <v>89</v>
       </c>
-    </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D92" s="2"/>
+    </row>
+    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C93">
         <v>90</v>
       </c>
-    </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D93" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C94">
         <v>91</v>
       </c>
-    </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C95">
         <v>92</v>
       </c>
-    </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D95" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C96">
         <v>93</v>
       </c>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D96" s="2"/>
+    </row>
+    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C97">
         <v>94</v>
       </c>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D97" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C98">
         <v>95</v>
       </c>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D98" s="2"/>
+    </row>
+    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C99">
         <v>96</v>
       </c>
-    </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D99" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C100">
         <v>97</v>
       </c>
-    </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D100" s="2"/>
+    </row>
+    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C101">
         <v>98</v>
       </c>
-    </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D101" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C102">
         <v>99</v>
       </c>
-    </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D102" s="2"/>
+    </row>
+    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C103">
         <v>100</v>
       </c>
-    </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D103" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C104">
         <v>101</v>
       </c>
-    </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D104" s="2"/>
+    </row>
+    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C105">
         <v>102</v>
       </c>
-    </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D105" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C106">
         <v>103</v>
       </c>
-    </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D106" s="2"/>
+    </row>
+    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C107">
         <v>104</v>
       </c>
-    </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D107" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C108">
         <v>105</v>
       </c>
-    </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D108" s="2"/>
+    </row>
+    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C109">
         <v>106</v>
       </c>
-    </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D109" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C110">
         <v>107</v>
       </c>
-    </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D110" s="2"/>
+    </row>
+    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C111">
         <v>108</v>
       </c>
-    </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D111" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C112">
         <v>109</v>
       </c>
-    </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D112" s="2"/>
+    </row>
+    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C113">
         <v>110</v>
       </c>
-    </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D113" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C114">
         <v>111</v>
       </c>
-    </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D114" s="2"/>
+    </row>
+    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C115">
         <v>112</v>
       </c>
-    </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D115" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C116">
         <v>113</v>
       </c>
-    </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D116" s="2"/>
+    </row>
+    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C117">
         <v>114</v>
       </c>
-    </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D117" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C118">
         <v>115</v>
       </c>
-    </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D118" s="2"/>
+    </row>
+    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C119">
         <v>116</v>
       </c>
-    </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D119" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C120">
         <v>117</v>
       </c>
-    </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D120" s="2"/>
+    </row>
+    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C121">
         <v>118</v>
       </c>
-    </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D121" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C122">
         <v>119</v>
       </c>
-    </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D122" s="2"/>
+    </row>
+    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C123">
         <v>120</v>
       </c>
-    </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D123" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C124">
         <v>121</v>
       </c>
-    </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D124" s="2"/>
+    </row>
+    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C125">
         <v>122</v>
       </c>
-    </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D125" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C126">
         <v>123</v>
       </c>
-    </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D126" s="2"/>
+    </row>
+    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C127">
         <v>124</v>
       </c>
-    </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D127" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="128" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C128">
         <v>125</v>
       </c>
-    </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D128" s="2"/>
+    </row>
+    <row r="129" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C129">
         <v>126</v>
       </c>
-    </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D129" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C130">
         <v>127</v>
       </c>
-    </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D130" s="2"/>
+    </row>
+    <row r="131" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C131">
         <v>128</v>
       </c>
-    </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D131" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="132" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C132">
         <v>129</v>
       </c>
-    </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D132" s="2"/>
+    </row>
+    <row r="133" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C133">
         <v>130</v>
       </c>
-    </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D133" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="134" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C134">
         <v>131</v>
       </c>
-    </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D134" s="2"/>
+    </row>
+    <row r="135" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C135">
         <v>132</v>
       </c>
-    </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D135" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C136">
         <v>133</v>
       </c>
-    </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D136" s="2"/>
+    </row>
+    <row r="137" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C137">
         <v>134</v>
       </c>
-    </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D137" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="138" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C138">
         <v>135</v>
       </c>
-    </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D138" s="2"/>
+    </row>
+    <row r="139" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C139">
         <v>136</v>
       </c>
-    </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D139" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="140" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C140">
         <v>137</v>
       </c>
-    </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D140" s="2"/>
+    </row>
+    <row r="141" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C141">
         <v>138</v>
       </c>
-    </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D141" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="142" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C142">
         <v>139</v>
       </c>
-    </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D142" s="2"/>
+    </row>
+    <row r="143" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C143">
         <v>140</v>
       </c>
-    </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D143" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="144" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C144">
         <v>141</v>
       </c>
-    </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D144" s="2"/>
+    </row>
+    <row r="145" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C145">
         <v>142</v>
       </c>
-    </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D145" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="146" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C146">
         <v>143</v>
       </c>
-    </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D146" s="2"/>
+    </row>
+    <row r="147" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C147">
         <v>144</v>
       </c>
-    </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D147" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="148" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C148">
         <v>145</v>
       </c>
-    </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D148" s="2"/>
+    </row>
+    <row r="149" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C149">
         <v>146</v>
       </c>
-    </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D149" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="150" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C150">
         <v>147</v>
       </c>
-    </row>
-    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D150" s="2"/>
+    </row>
+    <row r="151" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C151">
         <v>148</v>
       </c>
-    </row>
-    <row r="152" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D151" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="152" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C152">
         <v>149</v>
       </c>
-    </row>
-    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D152" s="2"/>
+    </row>
+    <row r="153" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C153">
         <v>150</v>
       </c>
-    </row>
-    <row r="154" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D153" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E153" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="154" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C154">
         <v>151</v>
       </c>
-    </row>
-    <row r="155" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D154" s="3"/>
+    </row>
+    <row r="155" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C155">
         <v>152</v>
       </c>
-    </row>
-    <row r="156" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D155" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="156" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C156">
         <v>153</v>
       </c>
-    </row>
-    <row r="157" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D156" s="3"/>
+    </row>
+    <row r="157" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C157">
         <v>154</v>
       </c>
-    </row>
-    <row r="158" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D157" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="158" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C158">
         <v>155</v>
       </c>
-    </row>
-    <row r="159" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D158" s="3"/>
+    </row>
+    <row r="159" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C159">
         <v>156</v>
       </c>
-    </row>
-    <row r="160" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D159" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="160" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C160">
         <v>157</v>
       </c>
-    </row>
-    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D160" s="3"/>
+    </row>
+    <row r="161" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C161">
         <v>158</v>
       </c>
-    </row>
-    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D161" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="162" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C162">
         <v>159</v>
       </c>
-    </row>
-    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D162" s="3"/>
+    </row>
+    <row r="163" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C163">
         <v>160</v>
       </c>
-    </row>
-    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D163" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="164" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C164">
         <v>161</v>
       </c>
-    </row>
-    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D164" s="3"/>
+    </row>
+    <row r="165" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C165">
         <v>162</v>
       </c>
-    </row>
-    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D165" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="166" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C166">
         <v>163</v>
       </c>
-    </row>
-    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D166" s="3"/>
+    </row>
+    <row r="167" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C167">
         <v>164</v>
       </c>
-    </row>
-    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D167" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="168" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C168">
         <v>165</v>
       </c>
-    </row>
-    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D168" s="3"/>
+    </row>
+    <row r="169" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C169">
         <v>166</v>
       </c>
-    </row>
-    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D169" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="170" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C170">
         <v>167</v>
       </c>
-    </row>
-    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D170" s="3"/>
+    </row>
+    <row r="171" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C171">
         <v>168</v>
       </c>
-    </row>
-    <row r="172" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D171" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="172" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C172">
         <v>169</v>
       </c>
-    </row>
-    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D172" s="3"/>
+    </row>
+    <row r="173" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C173">
         <v>170</v>
       </c>
-    </row>
-    <row r="174" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D173" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="174" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C174">
         <v>171</v>
       </c>
-    </row>
-    <row r="175" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D174" s="3"/>
+    </row>
+    <row r="175" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C175">
         <v>172</v>
       </c>
-    </row>
-    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D175" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="176" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C176">
         <v>173</v>
       </c>
-    </row>
-    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D176" s="3"/>
+    </row>
+    <row r="177" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C177">
         <v>174</v>
       </c>
-    </row>
-    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D177" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="178" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C178">
         <v>175</v>
       </c>
-    </row>
-    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D178" s="3"/>
+    </row>
+    <row r="179" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C179">
         <v>176</v>
       </c>
-    </row>
-    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D179" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="180" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C180">
         <v>177</v>
       </c>
-    </row>
-    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D180" s="3"/>
+    </row>
+    <row r="181" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C181">
         <v>178</v>
       </c>
-    </row>
-    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D181" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="182" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C182">
         <v>179</v>
       </c>
-    </row>
-    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D182" s="3"/>
+    </row>
+    <row r="183" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C183">
         <v>180</v>
       </c>
-    </row>
-    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D183" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="184" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C184">
         <v>181</v>
       </c>
-    </row>
-    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D184" s="3"/>
+    </row>
+    <row r="185" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C185">
         <v>182</v>
       </c>
-    </row>
-    <row r="186" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D185" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="186" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C186">
         <v>183</v>
       </c>
-    </row>
-    <row r="187" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D186" s="3"/>
+    </row>
+    <row r="187" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C187">
         <v>184</v>
       </c>
-    </row>
-    <row r="188" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D187" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="188" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C188">
         <v>185</v>
       </c>
-    </row>
-    <row r="189" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D188" s="3"/>
+    </row>
+    <row r="189" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C189">
         <v>186</v>
       </c>
-    </row>
-    <row r="190" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D189" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="190" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C190">
         <v>187</v>
       </c>
-    </row>
-    <row r="191" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D190" s="3"/>
+    </row>
+    <row r="191" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C191">
         <v>188</v>
       </c>
-    </row>
-    <row r="192" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D191" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="192" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C192">
         <v>189</v>
       </c>
-    </row>
-    <row r="193" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D192" s="3"/>
+    </row>
+    <row r="193" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C193">
         <v>190</v>
       </c>
-    </row>
-    <row r="194" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D193" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="194" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C194">
         <v>191</v>
       </c>
-    </row>
-    <row r="195" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D194" s="3"/>
+    </row>
+    <row r="195" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C195">
         <v>192</v>
       </c>
-    </row>
-    <row r="196" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D195" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="196" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C196">
         <v>193</v>
       </c>
-    </row>
-    <row r="197" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D196" s="3"/>
+    </row>
+    <row r="197" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C197">
         <v>194</v>
       </c>
-    </row>
-    <row r="198" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D197" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="198" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C198">
         <v>195</v>
       </c>
-    </row>
-    <row r="199" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D198" s="3"/>
+    </row>
+    <row r="199" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C199">
         <v>196</v>
       </c>
-    </row>
-    <row r="200" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D199" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="200" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C200">
         <v>197</v>
       </c>
-    </row>
-    <row r="201" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D200" s="3"/>
+    </row>
+    <row r="201" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C201">
         <v>198</v>
       </c>
-    </row>
-    <row r="202" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D201" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="202" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C202">
         <v>199</v>
       </c>
-    </row>
-    <row r="203" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D202" s="3"/>
+    </row>
+    <row r="203" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C203">
         <v>200</v>
       </c>
-    </row>
-    <row r="204" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D203" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="204" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C204">
         <v>201</v>
       </c>
-    </row>
-    <row r="205" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D204" s="3"/>
+    </row>
+    <row r="205" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C205">
         <v>202</v>
       </c>
-    </row>
-    <row r="206" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D205" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="206" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C206">
         <v>203</v>
       </c>
-    </row>
-    <row r="207" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D206" s="3"/>
+    </row>
+    <row r="207" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C207">
         <v>204</v>
       </c>
-    </row>
-    <row r="208" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D207" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="208" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C208">
         <v>205</v>
       </c>
-    </row>
-    <row r="209" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D208" s="3"/>
+    </row>
+    <row r="209" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C209">
         <v>206</v>
       </c>
-    </row>
-    <row r="210" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D209" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="210" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C210">
         <v>207</v>
       </c>
-    </row>
-    <row r="211" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D210" s="3"/>
+    </row>
+    <row r="211" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C211">
         <v>208</v>
       </c>
-    </row>
-    <row r="212" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D211" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="212" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C212">
         <v>209</v>
       </c>
-    </row>
-    <row r="213" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D212" s="3"/>
+    </row>
+    <row r="213" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C213">
         <v>210</v>
       </c>
-    </row>
-    <row r="214" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D213" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="214" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C214">
         <v>211</v>
       </c>
-    </row>
-    <row r="215" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D214" s="3"/>
+    </row>
+    <row r="215" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C215">
         <v>212</v>
       </c>
-    </row>
-    <row r="216" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D215" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="216" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C216">
         <v>213</v>
       </c>
-    </row>
-    <row r="217" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D216" s="3"/>
+    </row>
+    <row r="217" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C217">
         <v>214</v>
       </c>
-    </row>
-    <row r="218" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D217" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="218" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C218">
         <v>215</v>
       </c>
-    </row>
-    <row r="219" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D218" s="3"/>
+    </row>
+    <row r="219" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C219">
         <v>216</v>
       </c>
-    </row>
-    <row r="220" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D219" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="220" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C220">
         <v>217</v>
       </c>
-    </row>
-    <row r="221" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D220" s="3"/>
+    </row>
+    <row r="221" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C221">
         <v>218</v>
       </c>
-    </row>
-    <row r="222" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D221" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="222" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C222">
         <v>219</v>
       </c>
-    </row>
-    <row r="223" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D222" s="3"/>
+    </row>
+    <row r="223" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C223">
         <v>220</v>
       </c>
-    </row>
-    <row r="224" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D223" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="224" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C224">
         <v>221</v>
       </c>
-    </row>
-    <row r="225" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D224" s="3"/>
+    </row>
+    <row r="225" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C225">
         <v>222</v>
       </c>
-    </row>
-    <row r="226" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D225" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="226" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C226">
         <v>223</v>
       </c>
-    </row>
-    <row r="227" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D226" s="3"/>
+    </row>
+    <row r="227" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C227">
         <v>224</v>
       </c>
-    </row>
-    <row r="228" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D227" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="228" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C228">
         <v>225</v>
       </c>
-    </row>
-    <row r="229" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D228" s="3"/>
+    </row>
+    <row r="229" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C229">
         <v>226</v>
       </c>
-    </row>
-    <row r="230" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D229" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="230" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C230">
         <v>227</v>
       </c>
-    </row>
-    <row r="231" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D230" s="3"/>
+    </row>
+    <row r="231" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C231">
         <v>228</v>
       </c>
-    </row>
-    <row r="232" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D231" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="232" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C232">
         <v>229</v>
       </c>
-    </row>
-    <row r="233" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D232" s="3"/>
+    </row>
+    <row r="233" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C233">
         <v>230</v>
       </c>
-    </row>
-    <row r="234" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D233" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="234" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C234">
         <v>231</v>
       </c>
-    </row>
-    <row r="235" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D234" s="3"/>
+    </row>
+    <row r="235" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C235">
         <v>232</v>
       </c>
-    </row>
-    <row r="236" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D235" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="236" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C236">
         <v>233</v>
       </c>
-    </row>
-    <row r="237" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D236" s="3"/>
+    </row>
+    <row r="237" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C237">
         <v>234</v>
       </c>
-    </row>
-    <row r="238" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D237" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="238" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C238">
         <v>235</v>
       </c>
-    </row>
-    <row r="239" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D238" s="3"/>
+    </row>
+    <row r="239" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C239">
         <v>236</v>
       </c>
-    </row>
-    <row r="240" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D239" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="240" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C240">
         <v>237</v>
       </c>
-    </row>
-    <row r="241" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D240" s="3"/>
+    </row>
+    <row r="241" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C241">
         <v>238</v>
       </c>
-    </row>
-    <row r="242" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D241" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="242" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C242">
         <v>239</v>
       </c>
-    </row>
-    <row r="243" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D242" s="3"/>
+    </row>
+    <row r="243" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C243">
         <v>240</v>
       </c>
-    </row>
-    <row r="244" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D243" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="244" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C244">
         <v>241</v>
       </c>
-    </row>
-    <row r="245" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D244" s="3"/>
+    </row>
+    <row r="245" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C245">
         <v>242</v>
       </c>
-    </row>
-    <row r="246" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D245" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="246" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C246">
         <v>243</v>
       </c>
-    </row>
-    <row r="247" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D246" s="3"/>
+    </row>
+    <row r="247" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C247">
         <v>244</v>
       </c>
-    </row>
-    <row r="248" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D247" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="248" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C248">
         <v>245</v>
       </c>
-    </row>
-    <row r="249" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D248" s="3"/>
+    </row>
+    <row r="249" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C249">
         <v>246</v>
       </c>
-    </row>
-    <row r="250" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D249" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="250" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C250">
         <v>247</v>
       </c>
-    </row>
-    <row r="251" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D250" s="3"/>
+    </row>
+    <row r="251" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C251">
         <v>248</v>
       </c>
-    </row>
-    <row r="252" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D251" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="252" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C252">
         <v>249</v>
       </c>
-    </row>
-    <row r="253" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D252" s="3"/>
+    </row>
+    <row r="253" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C253">
         <v>250</v>
       </c>
     </row>
-    <row r="254" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C254">
         <v>251</v>
       </c>
     </row>
-    <row r="255" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C255">
         <v>252</v>
       </c>
     </row>
-    <row r="256" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C256">
         <v>253</v>
       </c>
@@ -1736,6 +2190,108 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="100">
+    <mergeCell ref="D245:D246"/>
+    <mergeCell ref="D247:D248"/>
+    <mergeCell ref="D249:D250"/>
+    <mergeCell ref="D251:D252"/>
+    <mergeCell ref="D233:D234"/>
+    <mergeCell ref="D235:D236"/>
+    <mergeCell ref="D237:D238"/>
+    <mergeCell ref="D239:D240"/>
+    <mergeCell ref="D241:D242"/>
+    <mergeCell ref="D243:D244"/>
+    <mergeCell ref="D221:D222"/>
+    <mergeCell ref="D223:D224"/>
+    <mergeCell ref="D225:D226"/>
+    <mergeCell ref="D227:D228"/>
+    <mergeCell ref="D229:D230"/>
+    <mergeCell ref="D231:D232"/>
+    <mergeCell ref="D209:D210"/>
+    <mergeCell ref="D211:D212"/>
+    <mergeCell ref="D213:D214"/>
+    <mergeCell ref="D215:D216"/>
+    <mergeCell ref="D217:D218"/>
+    <mergeCell ref="D219:D220"/>
+    <mergeCell ref="D197:D198"/>
+    <mergeCell ref="D199:D200"/>
+    <mergeCell ref="D201:D202"/>
+    <mergeCell ref="D203:D204"/>
+    <mergeCell ref="D205:D206"/>
+    <mergeCell ref="D207:D208"/>
+    <mergeCell ref="D185:D186"/>
+    <mergeCell ref="D187:D188"/>
+    <mergeCell ref="D189:D190"/>
+    <mergeCell ref="D191:D192"/>
+    <mergeCell ref="D193:D194"/>
+    <mergeCell ref="D195:D196"/>
+    <mergeCell ref="D173:D174"/>
+    <mergeCell ref="D175:D176"/>
+    <mergeCell ref="D177:D178"/>
+    <mergeCell ref="D179:D180"/>
+    <mergeCell ref="D181:D182"/>
+    <mergeCell ref="D183:D184"/>
+    <mergeCell ref="D161:D162"/>
+    <mergeCell ref="D163:D164"/>
+    <mergeCell ref="D165:D166"/>
+    <mergeCell ref="D167:D168"/>
+    <mergeCell ref="D169:D170"/>
+    <mergeCell ref="D171:D172"/>
+    <mergeCell ref="D149:D150"/>
+    <mergeCell ref="D151:D152"/>
+    <mergeCell ref="D153:D154"/>
+    <mergeCell ref="D155:D156"/>
+    <mergeCell ref="D157:D158"/>
+    <mergeCell ref="D159:D160"/>
+    <mergeCell ref="D137:D138"/>
+    <mergeCell ref="D139:D140"/>
+    <mergeCell ref="D141:D142"/>
+    <mergeCell ref="D143:D144"/>
+    <mergeCell ref="D145:D146"/>
+    <mergeCell ref="D147:D148"/>
+    <mergeCell ref="D125:D126"/>
+    <mergeCell ref="D127:D128"/>
+    <mergeCell ref="D129:D130"/>
+    <mergeCell ref="D131:D132"/>
+    <mergeCell ref="D133:D134"/>
+    <mergeCell ref="D135:D136"/>
+    <mergeCell ref="D113:D114"/>
+    <mergeCell ref="D115:D116"/>
+    <mergeCell ref="D117:D118"/>
+    <mergeCell ref="D119:D120"/>
+    <mergeCell ref="D121:D122"/>
+    <mergeCell ref="D123:D124"/>
+    <mergeCell ref="D101:D102"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="D107:D108"/>
+    <mergeCell ref="D109:D110"/>
+    <mergeCell ref="D111:D112"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="D93:D94"/>
+    <mergeCell ref="D95:D96"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="D99:D100"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="D87:D88"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="D63:D64"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>